<commit_message>
Student Onboarding 2nd commit
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -5,10 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationForm" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="EmailRegistration" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="SetPassword" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="LoginAsStudent" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="PersonalDetails" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -67,7 +71,7 @@
     <t xml:space="preserve">Thangaraj</t>
   </si>
   <si>
-    <t xml:space="preserve">priya.t+student1@icanio.com</t>
+    <t xml:space="preserve">priya.t+studentdemo1@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Na</t>
@@ -89,20 +93,88 @@
   </si>
   <si>
     <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t@icanio.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priya@2606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addressline1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addressline2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO 3/343, Korai road, Indhira nagar, Shanmugapuram, Ambattur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near to Kallikuppam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">india</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chennai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,6 +201,21 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,17 +260,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -195,6 +298,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFBCBEC4"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -311,97 +474,97 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>8122448784</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>2024</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="priya.t+student1@icanio.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="priya.t+studentdemo1@icanio.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -411,4 +574,222 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="Priya@2606"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="Priya@2606"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="priya.t+studentdemo1@icanio.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Priya@2606"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>34876</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>600099</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Student Onboarding 3rd commit
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationForm" sheetId="1" state="visible" r:id="rId3"/>
@@ -13,6 +13,8 @@
     <sheet name="SetPassword" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="LoginAsStudent" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="PersonalDetails" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="EdicationalDetails" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="AdditionalDetails" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -71,94 +73,184 @@
     <t xml:space="preserve">Thangaraj</t>
   </si>
   <si>
-    <t xml:space="preserve">priya.t+studentdemo1@icanio.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamil Na</t>
+    <t xml:space="preserve">priya.t+student31@icanio.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil Nadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chennai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1 Global Institute of Engineering and Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACHELOR OF ENGINEERING </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPUTER SCIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t@icanio.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priya@2606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addressline1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addressline2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO 3/343, Korai road, Indhira nagar, Shanmugapuram, Ambattur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near to Kallikuppam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">india</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chennai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schlname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthBoard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthstate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthcity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sethu Bhaskara MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Institute Of Open Schooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil</t>
   </si>
   <si>
     <t xml:space="preserve">Chenna</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo College of engineering 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BACHELOR OF ENGINEERING </t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPUTER SCIENCE ENGINEERING (CSE) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">June</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t@icanio.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priya@2606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addressline1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addressline2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO 3/343, Korai road, Indhira nagar, Shanmugapuram, Ambattur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near to Kallikuppam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">india</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tamil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chennai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">Bhartha vidhayalaya MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Of Secondary Education, Assam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careerobj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Category (GC) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports,Reading,Watching news and latest update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An excellent academic record, ability to understand and test software.</t>
   </si>
 </sst>
 </file>
@@ -169,7 +261,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -217,6 +309,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,7 +358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,15 +375,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,8 +584,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,7 +631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -563,9 +673,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="priya.t+studentdemo1@icanio.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -590,16 +697,16 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -634,10 +741,10 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -645,7 +752,7 @@
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -671,16 +778,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -694,8 +801,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="priya.t+studentdemo1@icanio.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Priya@2606"/>
+    <hyperlink ref="B2" r:id="rId1" display="Priya@2606"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -714,73 +820,255 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>34876</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>600099</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>34876</v>
+        <v>51</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>80</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>600099</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="O1:T2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in the student onboarding script
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -11,10 +11,9 @@
     <sheet name="RegistrationForm" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="EmailRegistration" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="SetPassword" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="LoginAsStudent" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="PersonalDetails" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="EdicationalDetails" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="AdditionalDetails" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="EducationalDetails" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="AdditionalDetails" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="PersonalDetails" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -73,7 +72,7 @@
     <t xml:space="preserve">Thangaraj</t>
   </si>
   <si>
-    <t xml:space="preserve">priya.t+student31@icanio.com</t>
+    <t xml:space="preserve">priya.t+student50@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -112,7 +111,94 @@
     <t xml:space="preserve">confirmPassword</t>
   </si>
   <si>
-    <t xml:space="preserve">emailid</t>
+    <t xml:space="preserve">schlname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthBoard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthstate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthcity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sethu Bhaskara MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Institute Of Open Schooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhartha vidhayalaya MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Of Secondary Education, Assam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careerobj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports,Reading,Watching news and latest update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An excellent academic record, ability to understand and test software.</t>
   </si>
   <si>
     <t xml:space="preserve">RegNo</t>
@@ -145,112 +231,13 @@
     <t xml:space="preserve">Female</t>
   </si>
   <si>
-    <t xml:space="preserve">NO 3/343, Korai road, Indhira nagar, Shanmugapuram, Ambattur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near to Kallikuppam</t>
+    <t xml:space="preserve">No:1 Gandhi Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMBT</t>
   </si>
   <si>
     <t xml:space="preserve">india</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tamil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chennai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schlname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthSchool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthBoard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthmonth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthyear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthpercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthstate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthcity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ugpercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sethu Bhaskara MHSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Institute Of Open Schooling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chenna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bhartha vidhayalaya MHSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Board Of Secondary Education, Assam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">religion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hobbies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lang1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lang2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">careerobj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General Category (GC) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sports,Reading,Watching news and latest update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An excellent academic record, ability to understand and test software.</t>
   </si>
 </sst>
 </file>
@@ -285,9 +272,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -304,16 +297,10 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFBCBEC4"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,30 +359,38 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -635,28 +630,28 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>8122448784</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -691,7 +686,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,13 +698,13 @@
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -735,7 +730,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,7 +744,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -775,7 +770,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -788,21 +783,96 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Priya@2606"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -818,76 +888,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>34876</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="true" ht="79" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>600099</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -905,170 +958,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>2017</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="D1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="O1:T2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O1" s="0" t="s">
+      <c r="G1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="7" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>6374266</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>36703</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="E2" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O2" s="8" t="s">
+      <c r="F2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>74</v>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>600099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Student onboarding coded for project and Internship
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -14,6 +14,8 @@
     <sheet name="EducationalDetails" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="AdditionalDetails" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="PersonalDetails" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="ProjectandInternship" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -66,13 +68,13 @@
     <t xml:space="preserve">endyear</t>
   </si>
   <si>
-    <t xml:space="preserve">Priya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thangaraj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t+student50@icanio.com</t>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t+studentdemo67@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -81,7 +83,7 @@
     <t xml:space="preserve">Chennai</t>
   </si>
   <si>
-    <t xml:space="preserve">A1 Global Institute of Engineering and Technology</t>
+    <t xml:space="preserve">Demo college of engineering 1</t>
   </si>
   <si>
     <t xml:space="preserve">BACHELOR OF ENGINEERING </t>
@@ -90,114 +92,120 @@
     <t xml:space="preserve">COMPUTER SCIENCE</t>
   </si>
   <si>
+    <t xml:space="preserve">Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t@icanio.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priya@2606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schlname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthBoard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthstate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twelfthcity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugpercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sethu Bhaskara MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Institute Of Open Schooling</t>
+  </si>
+  <si>
     <t xml:space="preserve">June</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t@icanio.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priya@2606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schlname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthSchool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthBoard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthmonth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthyear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthpercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthstate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelfthcity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ugpercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sethu Bhaskara MHSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Institute Of Open Schooling</t>
+    <t xml:space="preserve">Tamil Nad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhartha vidhayalaya MHSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Of Secondary Education, Assam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careerobj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports,Reading,Watching news and latest update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil</t>
   </si>
   <si>
-    <t xml:space="preserve">Chenna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bhartha vidhayalaya MHSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Board Of Secondary Education, Assam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">religion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hobbies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lang1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lang2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">careerobj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sports,Reading,Watching news and latest update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
     <t xml:space="preserve">An excellent academic record, ability to understand and test software.</t>
   </si>
   <si>
@@ -228,7 +236,7 @@
     <t xml:space="preserve">Pincode</t>
   </si>
   <si>
-    <t xml:space="preserve">Female</t>
+    <t xml:space="preserve">Male</t>
   </si>
   <si>
     <t xml:space="preserve">No:1 Gandhi Road</t>
@@ -237,18 +245,187 @@
     <t xml:space="preserve">CMBT</t>
   </si>
   <si>
-    <t xml:space="preserve">india</t>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projectTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startMonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endMOnth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projectcertificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interncompany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internstartMonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internstartYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internendMOnth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internendYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internfunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internrole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internindustry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interndescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internskill1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internskill2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internskill3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internskill4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internskill5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interncertificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAILESH COMPANY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For a project worked in the company for pratical experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Project certificate.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Techn parks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior Web Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got best performer in the Internship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle Sql Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Internship Certificate.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -269,11 +446,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -345,7 +517,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,19 +526,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,7 +546,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,8 +562,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -626,45 +806,45 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>8122448784</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -698,13 +878,13 @@
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -729,7 +909,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -744,7 +924,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -806,22 +986,22 @@
       <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -833,43 +1013,43 @@
         <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="O2" s="1" t="n">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -891,49 +1071,49 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="5" t="s">
         <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" s="9" customFormat="true" ht="79" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -961,64 +1141,64 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>66</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>6374266</v>
+        <v>889756</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>36703</v>
+        <v>36590</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>600099</v>
@@ -1033,4 +1213,241 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <v>2024</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Student Onboarding Work Experience
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -15,7 +15,7 @@
     <sheet name="AdditionalDetails" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="PersonalDetails" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="ProjectandInternship" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="WorkExperience" sheetId="8" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="158">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -68,13 +68,13 @@
     <t xml:space="preserve">endyear</t>
   </si>
   <si>
-    <t xml:space="preserve">Ram</t>
+    <t xml:space="preserve">Prem</t>
   </si>
   <si>
     <t xml:space="preserve">Kumar</t>
   </si>
   <si>
-    <t xml:space="preserve">priya.t+studentdemo67@icanio.com</t>
+    <t xml:space="preserve">priya.t+studentdemo68@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -414,6 +414,93 @@
   </si>
   <si>
     <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Internship Certificate.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobtitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Companyname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noticeperiod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awardname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AwardReceivedname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AwardDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bestperformancecertificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FrontEnd Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icanio Technologies 5.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">August</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend Developer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior Web Developer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Industry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need a career growth. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nodejs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javascript </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angularjs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For my work effect received a Best performer award.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Bestperformance certificate.jpg</t>
   </si>
 </sst>
 </file>
@@ -517,7 +604,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,10 +650,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,7 +843,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -848,6 +931,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="priya.t+studentdemo68@icanio.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1277,49 +1363,49 @@
       <c r="P1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1372,49 +1458,49 @@
       <c r="P2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="10" t="n">
         <v>2023</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="10" t="n">
         <v>2023</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AA2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AB2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AC2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AE2" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1434,14 +1520,115 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>45530</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
CoursesAndTraining and ProofDocuments script
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationForm" sheetId="1" state="visible" r:id="rId3"/>
@@ -16,6 +16,8 @@
     <sheet name="PersonalDetails" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="ProjectandInternship" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="WorkExperience" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="CoursesAndTraining" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="ProofAndDocument" sheetId="10" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="175">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -68,13 +70,13 @@
     <t xml:space="preserve">endyear</t>
   </si>
   <si>
-    <t xml:space="preserve">Prem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t+studentdemo68@icanio.com</t>
+    <t xml:space="preserve">Shanmugapriya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thangaraj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t+studentdemo76@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -236,7 +238,7 @@
     <t xml:space="preserve">Pincode</t>
   </si>
   <si>
-    <t xml:space="preserve">Male</t>
+    <t xml:space="preserve">Female</t>
   </si>
   <si>
     <t xml:space="preserve">No:1 Gandhi Road</t>
@@ -467,31 +469,28 @@
     <t xml:space="preserve">FrontEnd Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">Icanio Technologies 5.0 </t>
+    <t xml:space="preserve">Icanio Technologies 5.0</t>
   </si>
   <si>
     <t xml:space="preserve">August</t>
   </si>
   <si>
-    <t xml:space="preserve">Frontend Developer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Junior Web Developer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Industry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need a career growth. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nodejs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javascript </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angularjs </t>
+    <t xml:space="preserve">Frontend Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need a career growth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nodejs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angularjs</t>
   </si>
   <si>
     <t xml:space="preserve">Best Performance</t>
@@ -501,6 +500,60 @@
   </si>
   <si>
     <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Bestperformance certificate.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instituteName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coursestartmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coursestartyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courseendmonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courseendyear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CourseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CourseDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CourseCertificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besant Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java full stack developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To get the additional knowledge i undergone courses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\CourseCertificate.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDproof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addressproof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\DrivingLicense.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\ICANIO-10090\Pictures\Pancard.jpg</t>
   </si>
 </sst>
 </file>
@@ -512,7 +565,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -561,6 +614,13 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC77DBB"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -604,7 +664,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,6 +717,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +774,7 @@
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFC77DBB"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -842,8 +910,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,12 +999,49 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="priya.t+studentdemo68@icanio.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -995,7 +1100,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1144,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1226,7 +1331,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1263,10 +1368,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>889756</v>
+        <v>857556</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>36590</v>
+        <v>36489</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -1522,110 +1627,212 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="N2" s="11" t="n">
+        <v>45195</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.37"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>2022</v>
-      </c>
       <c r="E2" s="0" t="n">
-        <v>10</v>
+        <v>2023</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" s="0" t="s">
         <v>151</v>
       </c>
+      <c r="I2" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="J2" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="K2" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>45530</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>157</v>
+      <c r="K2" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Student onboarding script
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationForm" sheetId="1" state="visible" r:id="rId3"/>
@@ -70,13 +70,13 @@
     <t xml:space="preserve">endyear</t>
   </si>
   <si>
-    <t xml:space="preserve">Shanmugapriya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thangaraj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t+studentdemo76@icanio.com</t>
+    <t xml:space="preserve">Srikala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karthik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t+studentdemo83@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -664,7 +664,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -713,15 +713,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -910,8 +902,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,13 +981,13 @@
         <v>21</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
   </sheetData>
@@ -1017,24 +1009,24 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="10" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1143,8 +1135,8 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1207,7 +1199,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>68</v>
@@ -1228,7 +1220,7 @@
         <v>43</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>53</v>
@@ -1331,7 +1323,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1368,10 +1360,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>857556</v>
+        <v>197865</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>36489</v>
+        <v>36879</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -1752,86 +1744,86 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="16.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="4" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="10" t="n">
         <v>2023</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="10" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Student Roles Applying script 1st commit
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Students Onboarding.xlsx
+++ b/Excel/PluginLive Automation Students Onboarding.xlsx
@@ -70,13 +70,13 @@
     <t xml:space="preserve">endyear</t>
   </si>
   <si>
-    <t xml:space="preserve">Srikala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karthik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priya.t+studentdemo83@icanio.com</t>
+    <t xml:space="preserve">Vijay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.t+studentdemo90@icanio.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tamil Nadu</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">Pincode</t>
   </si>
   <si>
-    <t xml:space="preserve">Female</t>
+    <t xml:space="preserve">Male</t>
   </si>
   <si>
     <t xml:space="preserve">No:1 Gandhi Road</t>
@@ -903,7 +903,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1360,10 +1360,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>197865</v>
+        <v>12309876</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>36879</v>
+        <v>34967</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -1405,8 +1405,8 @@
   </sheetPr>
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1517,13 +1517,13 @@
         <v>43</v>
       </c>
       <c r="D2" s="10" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>106</v>
       </c>
       <c r="F2" s="10" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>105</v>
@@ -1562,13 +1562,13 @@
         <v>117</v>
       </c>
       <c r="S2" s="10" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="T2" s="10" t="s">
         <v>118</v>
       </c>
       <c r="U2" s="10" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>119</v>

</xml_diff>